<commit_message>
Fixed swapped size/express bug
</commit_message>
<xml_diff>
--- a/Cable Sizes.xlsx
+++ b/Cable Sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roneill\Documents\CRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B348B4F-5AC4-4072-82E5-627D48BA1C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9B5630-B8B4-4690-93C2-FEA4EAD4B196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="0" windowWidth="17775" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="840" windowWidth="17775" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -90,13 +90,13 @@
     <t>Lb Per Foot</t>
   </si>
   <si>
-    <t>SCALE CABLE</t>
-  </si>
-  <si>
-    <t>SCALE CABLE 2</t>
-  </si>
-  <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>SCALE 1</t>
+  </si>
+  <si>
+    <t>SCALE 2</t>
   </si>
 </sst>
 </file>
@@ -941,7 +941,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,24 +1086,24 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scaling + spiraling implemented
</commit_message>
<xml_diff>
--- a/Cable Sizes.xlsx
+++ b/Cable Sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roneill\Documents\CRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F483A69D-9ED4-4B6B-A186-27CF36DD3E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12D952E-E2AC-40A1-9D34-F470D751C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31410" yWindow="5775" windowWidth="11895" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31530" yWindow="2670" windowWidth="12150" windowHeight="20835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
scaling done, plotting not done
</commit_message>
<xml_diff>
--- a/Cable Sizes.xlsx
+++ b/Cable Sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{F12D952E-E2AC-40A1-9D34-F470D751C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EF09A7F-79F0-4328-A66E-557999E6408B}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{F12D952E-E2AC-40A1-9D34-F470D751C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{598CBACB-BCA0-4782-9D44-522D677FA849}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="390" windowWidth="14265" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -636,10 +636,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -942,7 +938,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2 Conductor Area Calculations
Visualization doesn't work yet, but area calculations are correct
</commit_message>
<xml_diff>
--- a/Cable Sizes.xlsx
+++ b/Cable Sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{F12D952E-E2AC-40A1-9D34-F470D751C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{598CBACB-BCA0-4782-9D44-522D677FA849}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{F12D952E-E2AC-40A1-9D34-F470D751C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67241EBC-1907-4076-A9DF-F37B6CD5B15F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13605" yWindow="630" windowWidth="14340" windowHeight="13485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Size</t>
   </si>
@@ -87,13 +87,16 @@
     <t>25C#14</t>
   </si>
   <si>
-    <t>Lb Per Foot</t>
-  </si>
-  <si>
-    <t>CABLE 1</t>
-  </si>
-  <si>
-    <t>CABLE 2</t>
+    <t>* 2 Conductor Cables Below *</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -577,9 +580,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -636,6 +642,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -935,21 +945,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -957,10 +968,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -968,10 +979,10 @@
         <v>1.3</v>
       </c>
       <c r="C2">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -979,10 +990,10 @@
         <v>1.175</v>
       </c>
       <c r="C3">
-        <v>0.73499999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -990,10 +1001,10 @@
         <v>1.4850000000000001</v>
       </c>
       <c r="C4">
-        <v>0.74299999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1001,10 +1012,10 @@
         <v>1.4850000000000001</v>
       </c>
       <c r="C5">
-        <v>0.74299999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1012,10 +1023,10 @@
         <v>0.99099999999999999</v>
       </c>
       <c r="C6">
-        <v>0.495</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1023,10 +1034,10 @@
         <v>1.232</v>
       </c>
       <c r="C7">
-        <v>0.71099999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1034,10 +1045,10 @@
         <v>1.27</v>
       </c>
       <c r="C8">
-        <v>0.76700000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1045,10 +1056,10 @@
         <v>1.3320000000000001</v>
       </c>
       <c r="C9">
-        <v>0.86499999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1056,10 +1067,10 @@
         <v>1.5069999999999999</v>
       </c>
       <c r="C10">
-        <v>1.284</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1067,10 +1078,10 @@
         <v>1.24</v>
       </c>
       <c r="C11">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1078,29 +1089,82 @@
         <v>0.9</v>
       </c>
       <c r="C12">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
+      <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C15">
+        <v>1.284</v>
+      </c>
+      <c r="D15">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="C16">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="D16">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="C17">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="D17">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="C18">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="D18">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made code able to be ran on local machine
</commit_message>
<xml_diff>
--- a/Cable Sizes.xlsx
+++ b/Cable Sizes.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roneill\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{F12D952E-E2AC-40A1-9D34-F470D751C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEAF038C-CFD9-4CE1-86C3-AFF35E7B5AF4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CAFC02-C5B8-4C3D-A4F1-8F3B7AA0AF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14190" yWindow="5475" windowWidth="14340" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6030" yWindow="1905" windowWidth="16545" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,27 +36,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Size</t>
   </si>
   <si>
-    <t>Diameter</t>
+    <t>Diameter (in)</t>
+  </si>
+  <si>
+    <t>Weight (lb/mft)</t>
+  </si>
+  <si>
+    <t>250 LSZH XHHW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250 THHN </t>
+  </si>
+  <si>
+    <t>500 THHN</t>
+  </si>
+  <si>
+    <t>500 LSZH XHHW</t>
+  </si>
+  <si>
+    <t>500 EPR XLPO</t>
+  </si>
+  <si>
+    <t>1C#4</t>
+  </si>
+  <si>
+    <t>1C#6</t>
+  </si>
+  <si>
+    <t>1C#9</t>
+  </si>
+  <si>
+    <t>1C#14</t>
+  </si>
+  <si>
+    <t>1C#16</t>
+  </si>
+  <si>
+    <t>1C#1/0</t>
+  </si>
+  <si>
+    <t>1C#2/0</t>
+  </si>
+  <si>
+    <t>1C#4/0</t>
+  </si>
+  <si>
+    <t>3C#4</t>
+  </si>
+  <si>
+    <t>3C#6</t>
+  </si>
+  <si>
+    <t>3C#9</t>
+  </si>
+  <si>
+    <t>7C#10</t>
+  </si>
+  <si>
+    <t>7C#12</t>
+  </si>
+  <si>
+    <t>7C#14</t>
+  </si>
+  <si>
+    <t>10C#14</t>
+  </si>
+  <si>
+    <t>12C#14</t>
+  </si>
+  <si>
+    <t>14C#14</t>
+  </si>
+  <si>
+    <t>19C#7</t>
+  </si>
+  <si>
+    <t>19C#14</t>
+  </si>
+  <si>
+    <t>25C#14</t>
+  </si>
+  <si>
+    <t>6PRC#19</t>
   </si>
   <si>
     <t>STAR QUAD</t>
   </si>
   <si>
-    <t>19C#14</t>
-  </si>
-  <si>
-    <t>7C#14</t>
-  </si>
-  <si>
-    <t>7C#12</t>
-  </si>
-  <si>
-    <t>7C#10</t>
+    <t>3 STAR QUAD</t>
+  </si>
+  <si>
+    <t>* 2 Conductor Cables Below *</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>2C#2</t>
   </si>
   <si>
     <t>2C#4</t>
@@ -67,43 +156,13 @@
   </si>
   <si>
     <t>2C#14</t>
-  </si>
-  <si>
-    <t>3C#4</t>
-  </si>
-  <si>
-    <t>3C#6</t>
-  </si>
-  <si>
-    <t>10C#14</t>
-  </si>
-  <si>
-    <t>12C#14</t>
-  </si>
-  <si>
-    <t>14C#14</t>
-  </si>
-  <si>
-    <t>25C#14</t>
-  </si>
-  <si>
-    <t>* 2 Conductor Cables Below *</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +295,12 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -580,11 +645,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -642,10 +711,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -945,18 +1010,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -968,202 +1032,417 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
+      <c r="A2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>1.3</v>
+        <v>0.71</v>
       </c>
       <c r="C2">
-        <v>960</v>
-      </c>
+        <v>880</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
+      <c r="A3" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>1.175</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="C3">
-        <v>735</v>
-      </c>
+        <v>851</v>
+      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="C4">
+        <v>1655</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>1.4850000000000001</v>
-      </c>
-      <c r="C4">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
       <c r="B5">
-        <v>1.4850000000000001</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="C5">
-        <v>743</v>
-      </c>
+        <v>1704</v>
+      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A6" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>0.99099999999999999</v>
+        <v>1.32</v>
       </c>
       <c r="C6">
-        <v>495</v>
-      </c>
+        <v>2000</v>
+      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
+      <c r="A7" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>1.232</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
-        <v>711</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>1.27</v>
+        <v>0.45</v>
       </c>
       <c r="C8">
-        <v>767</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>1.3320000000000001</v>
+        <v>0.37</v>
       </c>
       <c r="C9">
-        <v>865</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>1.5069999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="C10">
-        <v>1284</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>1.24</v>
+        <v>0.17</v>
       </c>
       <c r="C11">
-        <v>880</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="C12">
-        <v>860</v>
-      </c>
+        <v>490</v>
+      </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0.74</v>
+      </c>
+      <c r="C13">
+        <v>590</v>
+      </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>0.89</v>
+      </c>
+      <c r="C14">
+        <v>920</v>
+      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.8</v>
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>1.3</v>
       </c>
       <c r="C15">
-        <v>1.284</v>
-      </c>
-      <c r="D15">
-        <v>635</v>
+        <v>960</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.74</v>
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>1.175</v>
       </c>
       <c r="C16">
-        <v>1.1140000000000001</v>
-      </c>
-      <c r="D16">
-        <v>540</v>
+        <v>735</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.55100000000000005</v>
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>0.88500000000000001</v>
       </c>
       <c r="C17">
-        <v>0.83799999999999997</v>
-      </c>
-      <c r="D17">
-        <v>295</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>1.4850000000000001</v>
+      </c>
+      <c r="C18">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>1.4850000000000001</v>
+      </c>
+      <c r="C19">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="C20">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>1.232</v>
+      </c>
+      <c r="C21">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>1.27</v>
+      </c>
+      <c r="C22">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="C23">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="C24">
+        <v>204.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>1.5069999999999999</v>
+      </c>
+      <c r="C25">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>1.24</v>
+      </c>
+      <c r="C26">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>0.67</v>
+      </c>
+      <c r="C27">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>0.9</v>
+      </c>
+      <c r="C28">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>0.68</v>
+      </c>
+      <c r="C29">
+        <v>252.67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="C32">
+        <v>1.41</v>
+      </c>
+      <c r="D32">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="C33">
+        <v>1.284</v>
+      </c>
+      <c r="D33">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="C34">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="D34">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="C35">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="D35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="4">
         <v>0.48699999999999999</v>
       </c>
-      <c r="C18">
+      <c r="C36">
         <v>0.71699999999999997</v>
       </c>
-      <c r="D18">
+      <c r="D36">
         <v>201</v>
       </c>
     </row>
@@ -1173,37 +1452,309 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92E7ED7-8DAC-4334-B6A0-FB5C45401068}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9688d8ac-317d-4006-bb42-a7c83a467adb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090CFAD7B156278469C727DD80CE295F2" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2515fb5425965d1196afb2f18bfcce9f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xmlns:ns3="9688d8ac-317d-4006-bb42-a7c83a467adb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="060615b5e9a0f0b02fd967f87be859b5" ns2:_="" ns3:_="">
+    <xsd:import namespace="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
+    <xsd:import namespace="9688d8ac-317d-4006-bb42-a7c83a467adb"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{54e773fb-44d6-4cb2-82b4-3ebed2488986}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="3df27ed0-ad9d-4880-b677-86c7b6b9d64c">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9688d8ac-317d-4006-bb42-a7c83a467adb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="442eb2fe-09fc-4fcf-bf31-1833c4ad0ec6" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1351BEC7-B0D2-4C32-A843-FD5410CCB625}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA8C59D-6634-434D-BA9E-AC92A5B9A7C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9688d8ac-317d-4006-bb42-a7c83a467adb"/>
+    <ds:schemaRef ds:uri="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3B20A02-3E2B-495B-9F43-ADC3EA690AF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
+    <ds:schemaRef ds:uri="9688d8ac-317d-4006-bb42-a7c83a467adb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Laid down messenger files, can get to output file stage
</commit_message>
<xml_diff>
--- a/Cable Sizes.xlsx
+++ b/Cable Sizes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roneill\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CAFC02-C5B8-4C3D-A4F1-8F3B7AA0AF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{68CAFC02-C5B8-4C3D-A4F1-8F3B7AA0AF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49A069E9-396C-4C2E-A4D7-1E547D85FFCF}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="1905" windowWidth="16545" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="990" yWindow="1305" windowWidth="16545" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Size</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>2C#14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1027,7 @@
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1039,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1048,7 +1051,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1063,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1072,7 +1075,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1084,7 +1087,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1096,7 +1099,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1108,7 +1111,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1120,7 +1123,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1132,7 +1135,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1144,7 +1147,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1156,7 +1159,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1168,7 +1171,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1179,8 +1182,11 @@
         <v>590</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1192,7 +1198,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1203,7 +1209,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1453,15 +1459,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9688d8ac-317d-4006-bb42-a7c83a467adb">
@@ -1470,6 +1467,15 @@
     <TaxCatchAll xmlns="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1722,20 +1728,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1351BEC7-B0D2-4C32-A843-FD5410CCB625}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA8C59D-6634-434D-BA9E-AC92A5B9A7C0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9688d8ac-317d-4006-bb42-a7c83a467adb"/>
     <ds:schemaRef ds:uri="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1351BEC7-B0D2-4C32-A843-FD5410CCB625}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Ability to discern between 2 conductor cables with attribute
</commit_message>
<xml_diff>
--- a/Cable Sizes.xlsx
+++ b/Cable Sizes.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{F12D952E-E2AC-40A1-9D34-F470D751C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEAF038C-CFD9-4CE1-86C3-AFF35E7B5AF4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{850F8884-9124-4FDA-BF97-2EA8C3C8128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14190" yWindow="5475" windowWidth="14340" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,27 +36,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Size</t>
   </si>
   <si>
-    <t>Diameter</t>
+    <t>Diameter (in)</t>
+  </si>
+  <si>
+    <t>Weight (lb/mft)</t>
+  </si>
+  <si>
+    <t>250 LSZH XHHW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250 THHN </t>
+  </si>
+  <si>
+    <t>500 THHN</t>
+  </si>
+  <si>
+    <t>500 LSZH XHHW</t>
+  </si>
+  <si>
+    <t>500 EPR XLPO</t>
+  </si>
+  <si>
+    <t>1C#4</t>
+  </si>
+  <si>
+    <t>1C#6</t>
+  </si>
+  <si>
+    <t>1C#9</t>
+  </si>
+  <si>
+    <t>1C#14</t>
+  </si>
+  <si>
+    <t>1C#16</t>
+  </si>
+  <si>
+    <t>1C#1/0</t>
+  </si>
+  <si>
+    <t>1C#2/0</t>
+  </si>
+  <si>
+    <t>1C#4/0</t>
+  </si>
+  <si>
+    <t>3C#4</t>
+  </si>
+  <si>
+    <t>3C#6</t>
+  </si>
+  <si>
+    <t>3C#9</t>
+  </si>
+  <si>
+    <t>7C#10</t>
+  </si>
+  <si>
+    <t>7C#12</t>
+  </si>
+  <si>
+    <t>7C#14</t>
+  </si>
+  <si>
+    <t>10C#14</t>
+  </si>
+  <si>
+    <t>12C#14</t>
+  </si>
+  <si>
+    <t>14C#14</t>
+  </si>
+  <si>
+    <t>19C#7</t>
+  </si>
+  <si>
+    <t>19C#14</t>
+  </si>
+  <si>
+    <t>25C#14</t>
+  </si>
+  <si>
+    <t>6PRC#19</t>
   </si>
   <si>
     <t>STAR QUAD</t>
   </si>
   <si>
-    <t>19C#14</t>
-  </si>
-  <si>
-    <t>7C#14</t>
-  </si>
-  <si>
-    <t>7C#12</t>
-  </si>
-  <si>
-    <t>7C#10</t>
+    <t>3 STAR QUAD</t>
+  </si>
+  <si>
+    <t>* 2 Conductor Cables Below *</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>2C#2</t>
   </si>
   <si>
     <t>2C#4</t>
@@ -67,43 +156,13 @@
   </si>
   <si>
     <t>2C#14</t>
-  </si>
-  <si>
-    <t>3C#4</t>
-  </si>
-  <si>
-    <t>3C#6</t>
-  </si>
-  <si>
-    <t>10C#14</t>
-  </si>
-  <si>
-    <t>12C#14</t>
-  </si>
-  <si>
-    <t>14C#14</t>
-  </si>
-  <si>
-    <t>25C#14</t>
-  </si>
-  <si>
-    <t>* 2 Conductor Cables Below *</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +296,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="33">
@@ -580,12 +657,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -642,10 +718,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -945,22 +1017,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,202 +1039,435 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="C2" s="2">
+        <v>880</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="C3" s="2">
+        <v>851</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1655</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1704</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.32</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>220</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="C8" s="2">
+        <v>165</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="C9" s="2">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="C10" s="2">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="C11" s="2">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="C12" s="2">
+        <v>490</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="C13" s="2">
+        <v>590</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="C14" s="2">
+        <v>920</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>960</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.175</v>
+      </c>
+      <c r="C16" s="2">
+        <v>735</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="C17" s="2">
+        <v>395</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.4850000000000001</v>
+      </c>
+      <c r="C18" s="2">
+        <v>743</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>1.3</v>
-      </c>
-      <c r="C2">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>1.175</v>
-      </c>
-      <c r="C3">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+      <c r="B19" s="2">
         <v>1.4850000000000001</v>
       </c>
-      <c r="C4">
+      <c r="C19" s="2">
         <v>743</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1.4850000000000001</v>
-      </c>
-      <c r="C5">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
         <v>0.99099999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C20" s="2">
         <v>495</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2">
         <v>1.232</v>
       </c>
-      <c r="C7">
+      <c r="C21" s="2">
         <v>711</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
         <v>1.27</v>
       </c>
-      <c r="C8">
+      <c r="C22" s="2">
         <v>767</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2">
         <v>1.3320000000000001</v>
       </c>
-      <c r="C9">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
+      <c r="C23" s="2">
+        <v>856</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="C24" s="2">
+        <v>204.5</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2">
         <v>1.5069999999999999</v>
       </c>
-      <c r="C10">
+      <c r="C25" s="2">
         <v>1284</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2">
         <v>1.24</v>
       </c>
-      <c r="C11">
+      <c r="C26" s="2">
         <v>880</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="C27" s="2">
+        <v>165</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2">
         <v>0.9</v>
       </c>
-      <c r="C12">
+      <c r="C28" s="2">
         <v>860</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="C29" s="2">
+        <v>252.67</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="D32" s="2">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="2">
         <v>0.8</v>
       </c>
-      <c r="C15">
+      <c r="C33" s="2">
         <v>1.284</v>
       </c>
-      <c r="D15">
+      <c r="D33" s="2">
         <v>635</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="2">
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="2">
         <v>0.74</v>
       </c>
-      <c r="C16">
+      <c r="C34" s="2">
         <v>1.1140000000000001</v>
       </c>
-      <c r="D16">
+      <c r="D34" s="2">
         <v>540</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2">
+    <row r="35" spans="1:4">
+      <c r="A35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="2">
         <v>0.55100000000000005</v>
       </c>
-      <c r="C17">
+      <c r="C35" s="2">
         <v>0.83799999999999997</v>
       </c>
-      <c r="D17">
+      <c r="D35" s="2">
         <v>295</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2">
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="2">
         <v>0.48699999999999999</v>
       </c>
-      <c r="C18">
+      <c r="C36" s="2">
         <v>0.71699999999999997</v>
       </c>
-      <c r="D18">
+      <c r="D36" s="2">
         <v>201</v>
       </c>
     </row>
@@ -1173,37 +1477,283 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92E7ED7-8DAC-4334-B6A0-FB5C45401068}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090CFAD7B156278469C727DD80CE295F2" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2515fb5425965d1196afb2f18bfcce9f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xmlns:ns3="9688d8ac-317d-4006-bb42-a7c83a467adb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="060615b5e9a0f0b02fd967f87be859b5" ns2:_="" ns3:_="">
+    <xsd:import namespace="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
+    <xsd:import namespace="9688d8ac-317d-4006-bb42-a7c83a467adb"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{54e773fb-44d6-4cb2-82b4-3ebed2488986}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="3df27ed0-ad9d-4880-b677-86c7b6b9d64c">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9688d8ac-317d-4006-bb42-a7c83a467adb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="442eb2fe-09fc-4fcf-bf31-1833c4ad0ec6" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9688d8ac-317d-4006-bb42-a7c83a467adb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7147FE0-1B09-4361-BD37-A3B1FDF240F4}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18897649-DD57-4AD5-A81D-A3029D72B52A}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67DB52E1-1A1F-428B-BC03-B43E115ABD0B}"/>
 </file>
</xml_diff>

<commit_message>
Two conductors spaced correctly
</commit_message>
<xml_diff>
--- a/Cable Sizes.xlsx
+++ b/Cable Sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{850F8884-9124-4FDA-BF97-2EA8C3C8128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63B404FC-5520-4A4D-9196-B1D1E10F0D42}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{850F8884-9124-4FDA-BF97-2EA8C3C8128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8800525A-54E1-4744-8263-5609A1F73402}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="0" windowWidth="16350" windowHeight="10815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="0" windowWidth="11460" windowHeight="10710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,26 +1482,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9688d8ac-317d-4006-bb42-a7c83a467adb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090CFAD7B156278469C727DD80CE295F2" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2515fb5425965d1196afb2f18bfcce9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xmlns:ns3="9688d8ac-317d-4006-bb42-a7c83a467adb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="060615b5e9a0f0b02fd967f87be859b5" ns2:_="" ns3:_="">
     <xsd:import namespace="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
@@ -1750,10 +1730,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9688d8ac-317d-4006-bb42-a7c83a467adb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67DB52E1-1A1F-428B-BC03-B43E115ABD0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7147FE0-1B09-4361-BD37-A3B1FDF240F4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
+    <ds:schemaRef ds:uri="9688d8ac-317d-4006-bb42-a7c83a467adb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1770,20 +1781,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7147FE0-1B09-4361-BD37-A3B1FDF240F4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67DB52E1-1A1F-428B-BC03-B43E115ABD0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
-    <ds:schemaRef ds:uri="9688d8ac-317d-4006-bb42-a7c83a467adb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Logic to find new first conductor placement if second conductor cannot fit anywhere
</commit_message>
<xml_diff>
--- a/Cable Sizes.xlsx
+++ b/Cable Sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{850F8884-9124-4FDA-BF97-2EA8C3C8128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59DA1049-BABB-4CBE-AD3D-AC65AD1556DC}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{850F8884-9124-4FDA-BF97-2EA8C3C8128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D10AFF1C-8167-48C7-AE6B-397839F7E6EE}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="345" windowWidth="17235" windowHeight="12405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9630" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Size</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>4C#6</t>
   </si>
 </sst>
 </file>
@@ -721,10 +724,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1024,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,19 +1243,19 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2">
-        <v>1.4850000000000001</v>
+        <v>1.28</v>
       </c>
       <c r="C18" s="2">
-        <v>743</v>
+        <v>960</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2">
         <v>1.4850000000000001</v>
@@ -1268,215 +1267,227 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2">
-        <v>0.99099999999999999</v>
+        <v>1.4850000000000001</v>
       </c>
       <c r="C20" s="2">
-        <v>495</v>
+        <v>743</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1.232</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="C21" s="2">
-        <v>711</v>
+        <v>495</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>1.27</v>
+        <v>1.232</v>
       </c>
       <c r="C22" s="2">
-        <v>767</v>
+        <v>711</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2">
-        <v>1.3320000000000001</v>
+        <v>1.27</v>
       </c>
       <c r="C23" s="2">
-        <v>856</v>
+        <v>767</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2">
-        <v>0.59199999999999997</v>
+        <v>1.3320000000000001</v>
       </c>
       <c r="C24" s="2">
-        <v>204.5</v>
+        <v>856</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2">
-        <v>1.5069999999999999</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="C25" s="2">
-        <v>1284</v>
+        <v>204.5</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2">
-        <v>1.24</v>
+        <v>1.5069999999999999</v>
       </c>
       <c r="C26" s="2">
-        <v>880</v>
+        <v>1284</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="2">
-        <v>0.67</v>
+        <v>1.24</v>
       </c>
       <c r="C27" s="2">
-        <v>165</v>
+        <v>880</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2">
-        <v>0.9</v>
+        <v>0.67</v>
       </c>
       <c r="C28" s="2">
-        <v>860</v>
+        <v>165</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2">
-        <v>0.68</v>
+        <v>0.9</v>
       </c>
       <c r="C29" s="2">
-        <v>252.67</v>
+        <v>860</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="C30" s="2">
+        <v>252.67</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="2">
         <v>0.86</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C33" s="2">
         <v>1.41</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D33" s="2">
         <v>890</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="2">
-        <v>1.284</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="D33" s="2">
-        <v>635</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2">
-        <v>1.1140000000000001</v>
+        <v>1.284</v>
       </c>
       <c r="C34" s="2">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="D34" s="2">
-        <v>540</v>
+        <v>635</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2">
-        <v>0.83799999999999997</v>
+        <v>1.1140000000000001</v>
       </c>
       <c r="C35" s="2">
-        <v>0.55100000000000005</v>
+        <v>0.74</v>
       </c>
       <c r="D35" s="2">
-        <v>295</v>
+        <v>540</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="D36" s="2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B37" s="2">
         <v>0.71699999999999997</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C37" s="2">
         <v>0.48699999999999999</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D37" s="2">
         <v>201</v>
       </c>
     </row>
@@ -1487,26 +1498,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9688d8ac-317d-4006-bb42-a7c83a467adb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090CFAD7B156278469C727DD80CE295F2" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2515fb5425965d1196afb2f18bfcce9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xmlns:ns3="9688d8ac-317d-4006-bb42-a7c83a467adb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="060615b5e9a0f0b02fd967f87be859b5" ns2:_="" ns3:_="">
     <xsd:import namespace="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
@@ -1755,10 +1746,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9688d8ac-317d-4006-bb42-a7c83a467adb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3df27ed0-ad9d-4880-b677-86c7b6b9d64c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67DB52E1-1A1F-428B-BC03-B43E115ABD0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7147FE0-1B09-4361-BD37-A3B1FDF240F4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
+    <ds:schemaRef ds:uri="9688d8ac-317d-4006-bb42-a7c83a467adb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1775,20 +1797,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7147FE0-1B09-4361-BD37-A3B1FDF240F4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67DB52E1-1A1F-428B-BC03-B43E115ABD0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3df27ed0-ad9d-4880-b677-86c7b6b9d64c"/>
-    <ds:schemaRef ds:uri="9688d8ac-317d-4006-bb42-a7c83a467adb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>